<commit_message>
0223 Day2 AOS Shopping
</commit_message>
<xml_diff>
--- a/AOS Shopping 2/Default.xlsx
+++ b/AOS Shopping 2/Default.xlsx
@@ -14,6 +14,14 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1">
+  <si>
+    <t>Quantity</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
@@ -154,7 +162,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -162,13 +170,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -467,16 +491,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.41796875" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1"/>
+    <row customFormat="1">
+      <c t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row>
+      <c s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row>
+      <c s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row>
+      <c s="2">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
0223 Day 3 Ex 3a first part
</commit_message>
<xml_diff>
--- a/AOS Shopping 2/Default.xlsx
+++ b/AOS Shopping 2/Default.xlsx
@@ -15,9 +15,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="3">
   <si>
     <t>Quantity</t>
+  </si>
+  <si>
+    <t>AmountInCart</t>
+  </si>
+  <si>
+    <t>CHECKOUT ($539.98)</t>
   </si>
 </sst>
 </file>
@@ -162,7 +168,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -183,16 +189,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -491,37 +511,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
     <col min="1" max="1" width="9.41796875" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.078125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row customFormat="1">
       <c t="s">
         <v>0</v>
       </c>
+      <c t="s">
+        <v>1</v>
+      </c>
     </row>
     <row>
-      <c s="2">
+      <c s="3">
+        <v>2</v>
+      </c>
+      <c s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row>
-      <c s="2">
+      <c s="3">
         <v>3</v>
       </c>
+      <c s="2"/>
     </row>
     <row>
-      <c s="2">
+      <c s="3">
         <v>4</v>
       </c>
+      <c s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>